<commit_message>
updated xl file lab2
</commit_message>
<xml_diff>
--- a/Lab2/SIM_Lab2.xlsx
+++ b/Lab2/SIM_Lab2.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Storage</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Minimize</t>
+  </si>
+  <si>
+    <t>slope</t>
   </si>
 </sst>
 </file>
@@ -377,23 +380,76 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="8"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>correlation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" baseline="0"/>
+              <a:t> constraint and optimal function</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12333848594347314"/>
+          <c:y val="0.15090141915276778"/>
+          <c:w val="0.78041900715493162"/>
+          <c:h val="0.67422974842765171"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.720253812120649E-2"/>
+                  <c:y val="2.8933897579291462E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>'Primal Problem'!$A$23:$A$33</c:f>
               <c:numCache>
@@ -434,15 +490,10 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'Primal Problem'!$B$23:$B$33</c:f>
+              <c:f>'Primal Problem'!$C$23:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -481,7 +532,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -492,50 +543,309 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="138642944"/>
-        <c:axId val="449537152"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="138642944"/>
+        <c:axId val="360362496"/>
+        <c:axId val="360363072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="360362496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>raw</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> material units</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="449537152"/>
+        <c:crossAx val="360363072"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="449537152"/>
+        <c:axId val="360363072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>objective value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138642944"/>
+        <c:crossAx val="360362496"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>sensitivity analysis</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38736261206085126"/>
+          <c:y val="4.7709278440364905E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Primal Problem'!$A$23:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1665</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1695</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1710</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Primal Problem'!$B$23:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>2.1426666666666887</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1433333333333091</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1426666666666887</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1426666666666279</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1426666666666887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1433333333333091</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1426666666666887</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6153333333333042</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6153333333333648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6153333333333042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="648701056"/>
+        <c:axId val="367203392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="648701056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>raw material units</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="367203392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="367203392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>shadow price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="648701056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -552,20 +862,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>538443</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>146797</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>519393</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>70597</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33619</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>123262</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -575,6 +885,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>297236</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>105897</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1121,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1599,10 @@
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1267,7 +1610,7 @@
       <c r="A23">
         <v>1575</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>4335</v>
       </c>
     </row>
@@ -1276,6 +1619,10 @@
         <v>1590</v>
       </c>
       <c r="B24">
+        <f>(C24-C23)/(A24-A23)</f>
+        <v>2.1426666666666887</v>
+      </c>
+      <c r="C24">
         <v>4367.1400000000003</v>
       </c>
     </row>
@@ -1284,6 +1631,10 @@
         <v>1605</v>
       </c>
       <c r="B25">
+        <f>(C25-C24)/(A25-A24)</f>
+        <v>2.1433333333333091</v>
+      </c>
+      <c r="C25">
         <v>4399.29</v>
       </c>
     </row>
@@ -1292,6 +1643,10 @@
         <v>1620</v>
       </c>
       <c r="B26">
+        <f>(C26-C25)/(A26-A25)</f>
+        <v>2.1426666666666887</v>
+      </c>
+      <c r="C26">
         <v>4431.43</v>
       </c>
     </row>
@@ -1300,6 +1655,10 @@
         <v>1635</v>
       </c>
       <c r="B27">
+        <f>(C27-C26)/(A27-A26)</f>
+        <v>2.1426666666666279</v>
+      </c>
+      <c r="C27">
         <v>4463.57</v>
       </c>
     </row>
@@ -1308,6 +1667,10 @@
         <v>1650</v>
       </c>
       <c r="B28">
+        <f>(C28-C27)/(A28-A27)</f>
+        <v>2.1426666666666887</v>
+      </c>
+      <c r="C28">
         <v>4495.71</v>
       </c>
     </row>
@@ -1316,6 +1679,10 @@
         <v>1665</v>
       </c>
       <c r="B29">
+        <f>(C29-C28)/(A29-A28)</f>
+        <v>2.1433333333333091</v>
+      </c>
+      <c r="C29">
         <v>4527.8599999999997</v>
       </c>
     </row>
@@ -1324,6 +1691,10 @@
         <v>1680</v>
       </c>
       <c r="B30">
+        <f>(C30-C29)/(A30-A29)</f>
+        <v>2.1426666666666887</v>
+      </c>
+      <c r="C30">
         <v>4560</v>
       </c>
     </row>
@@ -1332,6 +1703,10 @@
         <v>1695</v>
       </c>
       <c r="B31">
+        <f>(C31-C30)/(A31-A30)</f>
+        <v>1.6153333333333042</v>
+      </c>
+      <c r="C31">
         <v>4584.2299999999996</v>
       </c>
     </row>
@@ -1340,14 +1715,22 @@
         <v>1710</v>
       </c>
       <c r="B32">
+        <f>(C32-C31)/(A32-A31)</f>
+        <v>1.6153333333333648</v>
+      </c>
+      <c r="C32">
         <v>4608.46</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1725</v>
       </c>
       <c r="B33">
+        <f>(C33-C32)/(A33-A32)</f>
+        <v>1.6153333333333042</v>
+      </c>
+      <c r="C33">
         <v>4632.6899999999996</v>
       </c>
     </row>

</xml_diff>